<commit_message>
Sprint : PPG Sprint 6    state : Finished
</commit_message>
<xml_diff>
--- a/ECU1/TestCases/ECU1_EntranceGate_TestCases.xlsx
+++ b/ECU1/TestCases/ECU1_EntranceGate_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\COURSES\Learn-in-Depth\Repo\Unit_10_SecondTermProject\ECU1\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE616C62-15C2-4000-97D2-446AA47F3711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB74B48-8932-432A-8782-6919C3ED77A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FBA70518-CB10-42FD-A195-A863F06D5FAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="102">
   <si>
     <t>Test ID</t>
   </si>
@@ -394,6 +394,29 @@
   </si>
   <si>
     <t>TC_Gate_15</t>
+  </si>
+  <si>
+    <t>Validate functionality of LEDs  (Entrnce Gate)</t>
+  </si>
+  <si>
+    <t>TC_Gate_16</t>
+  </si>
+  <si>
+    <t>TC_Gate_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that Green Led </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that Red Led </t>
+  </si>
+  <si>
+    <t>Green Led on 
+Red Led off</t>
+  </si>
+  <si>
+    <t>Green Led off 
+Red Led on</t>
   </si>
 </sst>
 </file>
@@ -478,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -491,18 +514,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,17 +522,266 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="112">
+  <dxfs count="136">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1954,13 +2214,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB1C29D-A9BC-4A81-B2AF-DC978394A8D6}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="13" customWidth="1"/>
+    <col min="1" max="1" width="18" style="8" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" hidden="1" customWidth="1"/>
@@ -1976,7 +2236,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2014,7 +2274,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B2" t="s">
@@ -2047,10 +2307,10 @@
       <c r="L2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="5"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="3" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -2081,10 +2341,10 @@
       <c r="L3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="6"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -2115,10 +2375,10 @@
       <c r="L4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -2149,10 +2409,10 @@
       <c r="L5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -2183,10 +2443,10 @@
       <c r="L6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="6"/>
+      <c r="M6" s="12"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2201,7 +2461,7 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B8" t="s">
@@ -2236,7 +2496,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2251,7 +2511,7 @@
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B10" t="s">
@@ -2286,7 +2546,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11" t="s">
         <v>53</v>
       </c>
@@ -2319,7 +2579,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2334,7 +2594,7 @@
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B13" t="s">
@@ -2369,7 +2629,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2384,7 +2644,7 @@
       <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B15" t="s">
@@ -2419,7 +2679,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="A16" s="10"/>
       <c r="B16" t="s">
         <v>68</v>
       </c>
@@ -2452,7 +2712,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
+      <c r="A17" s="10"/>
       <c r="B17" t="s">
         <v>69</v>
       </c>
@@ -2485,7 +2745,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="10"/>
       <c r="B18" t="s">
         <v>70</v>
       </c>
@@ -2518,7 +2778,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2533,7 +2793,7 @@
       <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B20" t="s">
@@ -2568,7 +2828,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="10"/>
       <c r="B21" t="s">
         <v>94</v>
       </c>
@@ -2597,6 +2857,89 @@
         <v>14</v>
       </c>
       <c r="L21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2604,7 +2947,8 @@
       <c r="F26" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="M2:M6"/>
     <mergeCell ref="A2:A6"/>
@@ -2613,6 +2957,90 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:M1 A2:G2 I2:M2 A3:M5 A7:M7 A6:G6 I6:M6 I8:M8 A8:E8 G8 F26 A9:M9 A10:E10 B11:E11 A12:M12 F10:L11">
+    <cfRule type="cellIs" dxfId="135" priority="157" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="158" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="159" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="160" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="cellIs" dxfId="131" priority="145" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="146" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="147" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="148" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="cellIs" dxfId="127" priority="141" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="142" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="143" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="144" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="123" priority="137" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="138" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="139" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="140" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="119" priority="133" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="134" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="135" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="136" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="115" priority="129" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="130" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="131" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="132" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
     <cfRule type="cellIs" dxfId="111" priority="125" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2626,63 +3054,63 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="107" priority="113" operator="equal">
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="107" priority="121" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="122" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="123" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="124" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="103" priority="109" operator="equal">
+  <conditionalFormatting sqref="K13">
+    <cfRule type="cellIs" dxfId="103" priority="117" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="118" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="119" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="120" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="99" priority="105" operator="equal">
+  <conditionalFormatting sqref="J13">
+    <cfRule type="cellIs" dxfId="99" priority="113" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="114" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="115" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="116" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="95" priority="101" operator="equal">
+  <conditionalFormatting sqref="A14:M14">
+    <cfRule type="cellIs" dxfId="95" priority="109" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="110" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="111" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="112" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
+  <conditionalFormatting sqref="A15">
     <cfRule type="cellIs" dxfId="91" priority="97" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2696,7 +3124,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G13">
+  <conditionalFormatting sqref="B15:B18">
     <cfRule type="cellIs" dxfId="87" priority="93" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2710,7 +3138,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
+  <conditionalFormatting sqref="C15">
     <cfRule type="cellIs" dxfId="83" priority="89" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2724,7 +3152,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
+  <conditionalFormatting sqref="E15:E18">
     <cfRule type="cellIs" dxfId="79" priority="85" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2738,7 +3166,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
+  <conditionalFormatting sqref="F15:F18">
     <cfRule type="cellIs" dxfId="75" priority="81" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2752,7 +3180,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:M14">
+  <conditionalFormatting sqref="I15:I18">
     <cfRule type="cellIs" dxfId="71" priority="77" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2766,119 +3194,119 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="67" priority="65" operator="equal">
+  <conditionalFormatting sqref="A19:M19">
+    <cfRule type="cellIs" dxfId="67" priority="73" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="74" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="75" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B18">
-    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="62" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="63" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="64" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E18">
-    <cfRule type="cellIs" dxfId="55" priority="53" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F18">
-    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15:I18">
-    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:M19">
-    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="76" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="69" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="71" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="72" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:B21">
+    <cfRule type="cellIs" dxfId="59" priority="65" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="67" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="68" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E21">
+    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="63" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="64" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20:F21">
+    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="56" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="51" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="cellIs" dxfId="43" priority="45" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="46" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="47" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="48" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:K18">
+    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="44" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20:K21">
     <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2892,7 +3320,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E21">
+  <conditionalFormatting sqref="A22:M22">
     <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2906,7 +3334,21 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F21">
+  <conditionalFormatting sqref="A23">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:B24">
     <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2920,7 +3362,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
+  <conditionalFormatting sqref="E23:E24">
     <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2934,7 +3376,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
+  <conditionalFormatting sqref="F23:F24">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2948,7 +3390,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J15:K18">
+  <conditionalFormatting sqref="I23">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2962,7 +3404,21 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J20:K21">
+  <conditionalFormatting sqref="I24">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J23:K24">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>

</xml_diff>